<commit_message>
Can now have empty spaces in timesheet
</commit_message>
<xml_diff>
--- a/files/sample_timesheet.xlsx
+++ b/files/sample_timesheet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
   <si>
     <t xml:space="preserve">Date (DD/MM/YYYY)</t>
   </si>
@@ -49,16 +49,16 @@
     <t xml:space="preserve">Dimensions Integrations Training</t>
   </si>
   <si>
+    <t xml:space="preserve">Did other thing</t>
+  </si>
+  <si>
     <t xml:space="preserve">Did thing</t>
   </si>
   <si>
-    <t xml:space="preserve">Internal_Activity</t>
+    <t xml:space="preserve">Hello</t>
   </si>
   <si>
-    <t xml:space="preserve">English</t>
-  </si>
-  <si>
-    <t xml:space="preserve">English lesson</t>
+    <t xml:space="preserve">Hello 2</t>
   </si>
 </sst>
 </file>
@@ -183,11 +183,11 @@
   </sheetPr>
   <dimension ref="A1:G1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="34.59"/>
@@ -223,16 +223,16 @@
       <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="n">
+      <c r="C2" s="0" t="n">
         <v>152</v>
       </c>
-      <c r="D2" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="D2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="0" t="s">
         <v>9</v>
       </c>
     </row>
@@ -240,44 +240,103 @@
       <c r="A3" s="1" t="n">
         <v>44627</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="2"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>44627</v>
+      </c>
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <v>44627</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="n">
+        <v>44627</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="n">
+        <v>44627</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="n">
+        <v>44627</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="n">
+        <v>44627</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>152</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="E3" s="0" t="s">
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="n">
+        <v>44628</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>152</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="0" t="s">
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="n">
+        <v>44628</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="n">
+        <v>44628</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="n">
+        <v>44628</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="2" t="n">
+        <v>152</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4"/>
-    </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4"/>
-    </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4"/>
-    </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4"/>
-    </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4"/>

</xml_diff>

<commit_message>
Included non jira entry in sample timesheet
</commit_message>
<xml_diff>
--- a/files/sample_timesheet.xlsx
+++ b/files/sample_timesheet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t xml:space="preserve">Date (DD/MM/YYYY)</t>
   </si>
@@ -43,22 +43,19 @@
     <t xml:space="preserve">JiraIgnore</t>
   </si>
   <si>
-    <t xml:space="preserve">ATWGBTRN</t>
+    <t xml:space="preserve">SAMPLE</t>
   </si>
   <si>
-    <t xml:space="preserve">Dimensions Integrations Training</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Did other thing</t>
+    <t xml:space="preserve">Sample Jira Entry</t>
   </si>
   <si>
     <t xml:space="preserve">Did thing</t>
   </si>
   <si>
-    <t xml:space="preserve">Hello</t>
+    <t xml:space="preserve">Sample Non Jira Entry</t>
   </si>
   <si>
-    <t xml:space="preserve">Hello 2</t>
+    <t xml:space="preserve">Did other thing</t>
   </si>
 </sst>
 </file>
@@ -184,10 +181,10 @@
   <dimension ref="A1:G1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="34.59"/>
@@ -224,7 +221,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>152</v>
+        <v>123</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>1</v>
@@ -238,118 +235,36 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
-        <v>44627</v>
+        <v>44628</v>
       </c>
       <c r="B3" s="2"/>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
-        <v>44627</v>
+      <c r="D3" s="0" t="n">
+        <v>3.5</v>
       </c>
-      <c r="G4" s="3"/>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
-        <v>44627</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="n">
-        <v>44627</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="n">
-        <v>44627</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="n">
-        <v>44627</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="n">
-        <v>44627</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="2" t="n">
-        <v>152</v>
-      </c>
-      <c r="D9" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9" s="2" t="s">
+      <c r="E3" s="0" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="n">
-        <v>44628</v>
+      <c r="F3" s="0" t="s">
+        <v>11</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="2" t="n">
-        <v>152</v>
-      </c>
-      <c r="D10" s="0" t="n">
+      <c r="G3" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F10" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="n">
-        <v>44628</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="n">
-        <v>44628</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="n">
-        <v>44628</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="2" t="n">
-        <v>152</v>
-      </c>
-      <c r="D13" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F13" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="4"/>
-    </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="4"/>
-    </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="4"/>
-    </row>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="4"/>
-    </row>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4"/>
     </row>

</xml_diff>

<commit_message>
Mostly finished with V0.2.0 - Design changes, performance improvement, less classes / complexity
</commit_message>
<xml_diff>
--- a/files/sample_timesheet.xlsx
+++ b/files/sample_timesheet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t xml:space="preserve">Date (DD/MM/YYYY)</t>
   </si>
@@ -31,41 +31,31 @@
     <t xml:space="preserve">Issue</t>
   </si>
   <si>
-    <t xml:space="preserve">Hours</t>
+    <t xml:space="preserve">TimeSpent</t>
   </si>
   <si>
-    <t xml:space="preserve">Title</t>
+    <t xml:space="preserve">TimeRemaining</t>
   </si>
   <si>
-    <t xml:space="preserve">Description</t>
+    <t xml:space="preserve">Comment</t>
   </si>
   <si>
-    <t xml:space="preserve">JiraIgnore</t>
+    <t xml:space="preserve">Ignore</t>
   </si>
   <si>
-    <t xml:space="preserve">SAMPLE</t>
+    <t xml:space="preserve">ATWGBTRN</t>
   </si>
   <si>
-    <t xml:space="preserve">Sample Jira Entry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Did thing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sample Non Jira Entry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Did other thing</t>
+    <t xml:space="preserve">TEST</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="dd\/mm\/yyyy"/>
-    <numFmt numFmtId="166" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="165" formatCode="mm/dd/yy"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -145,15 +135,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -178,3041 +168,3005 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G1000"/>
+  <dimension ref="A1:G999"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.71484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="34.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="30.27"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
-        <v>44627</v>
+      <c r="A2" s="2" t="n">
+        <v>44426</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>123</v>
+        <v>247</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="F2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
-        <v>44628</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="D3" s="0" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="4"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4"/>
     </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4"/>
     </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4"/>
     </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4"/>
     </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4"/>
     </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4"/>
     </row>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4"/>
     </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4"/>
     </row>
-    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="4"/>
     </row>
-    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4"/>
     </row>
-    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="4"/>
     </row>
-    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4"/>
     </row>
-    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4"/>
     </row>
-    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4"/>
     </row>
-    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="4"/>
     </row>
-    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4"/>
     </row>
-    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="4"/>
     </row>
-    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="4"/>
     </row>
-    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="4"/>
     </row>
-    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="4"/>
     </row>
-    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="4"/>
     </row>
-    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="4"/>
     </row>
-    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="4"/>
     </row>
-    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="4"/>
     </row>
-    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="4"/>
     </row>
-    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="4"/>
     </row>
-    <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="4"/>
     </row>
-    <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="4"/>
     </row>
-    <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="4"/>
     </row>
-    <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="4"/>
     </row>
-    <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="4"/>
     </row>
-    <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="4"/>
     </row>
-    <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="4"/>
     </row>
-    <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="4"/>
     </row>
-    <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="4"/>
     </row>
-    <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="4"/>
     </row>
-    <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="4"/>
     </row>
-    <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="4"/>
     </row>
-    <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="4"/>
     </row>
-    <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="4"/>
     </row>
-    <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="4"/>
     </row>
-    <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="4"/>
     </row>
-    <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="4"/>
     </row>
-    <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="4"/>
     </row>
-    <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="4"/>
     </row>
-    <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="4"/>
     </row>
-    <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="4"/>
     </row>
-    <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="4"/>
     </row>
-    <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="4"/>
     </row>
-    <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="4"/>
     </row>
-    <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="4"/>
     </row>
-    <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="4"/>
     </row>
-    <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="4"/>
     </row>
-    <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="4"/>
     </row>
-    <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="4"/>
     </row>
-    <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="4"/>
     </row>
-    <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="4"/>
     </row>
-    <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="4"/>
     </row>
-    <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="4"/>
     </row>
-    <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="4"/>
     </row>
-    <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="4"/>
     </row>
-    <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="4"/>
     </row>
-    <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="4"/>
     </row>
-    <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="4"/>
     </row>
-    <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="4"/>
     </row>
-    <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="4"/>
     </row>
-    <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="4"/>
     </row>
-    <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="4"/>
     </row>
-    <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="4"/>
     </row>
-    <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="4"/>
     </row>
-    <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="4"/>
     </row>
-    <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="4"/>
     </row>
-    <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="4"/>
     </row>
-    <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="4"/>
     </row>
-    <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="4"/>
     </row>
-    <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="4"/>
     </row>
-    <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="4"/>
     </row>
-    <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="4"/>
     </row>
-    <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="4"/>
     </row>
-    <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="4"/>
     </row>
-    <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="4"/>
     </row>
-    <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="4"/>
     </row>
-    <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="4"/>
     </row>
-    <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="4"/>
     </row>
-    <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="4"/>
     </row>
-    <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="4"/>
     </row>
-    <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="4"/>
     </row>
-    <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="4"/>
     </row>
-    <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="4"/>
     </row>
-    <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="4"/>
     </row>
-    <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="4"/>
     </row>
-    <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="4"/>
     </row>
-    <row r="110" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="4"/>
     </row>
-    <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="4"/>
     </row>
-    <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="4"/>
     </row>
-    <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="4"/>
     </row>
-    <row r="114" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="4"/>
     </row>
-    <row r="115" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="4"/>
     </row>
-    <row r="116" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="4"/>
     </row>
-    <row r="117" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="4"/>
     </row>
-    <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="4"/>
     </row>
-    <row r="119" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="4"/>
     </row>
-    <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="4"/>
     </row>
-    <row r="121" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="4"/>
     </row>
-    <row r="122" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="4"/>
     </row>
-    <row r="123" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="4"/>
     </row>
-    <row r="124" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="4"/>
     </row>
-    <row r="125" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="4"/>
     </row>
-    <row r="126" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="4"/>
     </row>
-    <row r="127" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="4"/>
     </row>
-    <row r="128" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="4"/>
     </row>
-    <row r="129" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="4"/>
     </row>
-    <row r="130" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="4"/>
     </row>
-    <row r="131" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="4"/>
     </row>
-    <row r="132" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="4"/>
     </row>
-    <row r="133" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="4"/>
     </row>
-    <row r="134" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="4"/>
     </row>
-    <row r="135" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="4"/>
     </row>
-    <row r="136" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="4"/>
     </row>
-    <row r="137" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="4"/>
     </row>
-    <row r="138" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="4"/>
     </row>
-    <row r="139" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="4"/>
     </row>
-    <row r="140" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="4"/>
     </row>
-    <row r="141" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="4"/>
     </row>
-    <row r="142" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="4"/>
     </row>
-    <row r="143" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="4"/>
     </row>
-    <row r="144" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="4"/>
     </row>
-    <row r="145" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="4"/>
     </row>
-    <row r="146" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="4"/>
     </row>
-    <row r="147" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="4"/>
     </row>
-    <row r="148" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="4"/>
     </row>
-    <row r="149" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="4"/>
     </row>
-    <row r="150" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="4"/>
     </row>
-    <row r="151" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="4"/>
     </row>
-    <row r="152" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="4"/>
     </row>
-    <row r="153" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="4"/>
     </row>
-    <row r="154" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="4"/>
     </row>
-    <row r="155" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="4"/>
     </row>
-    <row r="156" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="4"/>
     </row>
-    <row r="157" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="4"/>
     </row>
-    <row r="158" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="4"/>
     </row>
-    <row r="159" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="4"/>
     </row>
-    <row r="160" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="4"/>
     </row>
-    <row r="161" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="4"/>
     </row>
-    <row r="162" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="4"/>
     </row>
-    <row r="163" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="4"/>
     </row>
-    <row r="164" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="4"/>
     </row>
-    <row r="165" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="4"/>
     </row>
-    <row r="166" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="4"/>
     </row>
-    <row r="167" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="4"/>
     </row>
-    <row r="168" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="4"/>
     </row>
-    <row r="169" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="4"/>
     </row>
-    <row r="170" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="4"/>
     </row>
-    <row r="171" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="4"/>
     </row>
-    <row r="172" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="4"/>
     </row>
-    <row r="173" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="4"/>
     </row>
-    <row r="174" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="4"/>
     </row>
-    <row r="175" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="4"/>
     </row>
-    <row r="176" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="4"/>
     </row>
-    <row r="177" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="4"/>
     </row>
-    <row r="178" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="4"/>
     </row>
-    <row r="179" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="4"/>
     </row>
-    <row r="180" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="4"/>
     </row>
-    <row r="181" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="4"/>
     </row>
-    <row r="182" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="4"/>
     </row>
-    <row r="183" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="4"/>
     </row>
-    <row r="184" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="4"/>
     </row>
-    <row r="185" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="4"/>
     </row>
-    <row r="186" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="4"/>
     </row>
-    <row r="187" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="4"/>
     </row>
-    <row r="188" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="4"/>
     </row>
-    <row r="189" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="4"/>
     </row>
-    <row r="190" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="4"/>
     </row>
-    <row r="191" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="4"/>
     </row>
-    <row r="192" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="4"/>
     </row>
-    <row r="193" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="4"/>
     </row>
-    <row r="194" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="4"/>
     </row>
-    <row r="195" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="4"/>
     </row>
-    <row r="196" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="196" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="4"/>
     </row>
-    <row r="197" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="197" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="4"/>
     </row>
-    <row r="198" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="4"/>
     </row>
-    <row r="199" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="4"/>
     </row>
-    <row r="200" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="4"/>
     </row>
-    <row r="201" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="4"/>
     </row>
-    <row r="202" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="4"/>
     </row>
-    <row r="203" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="4"/>
     </row>
-    <row r="204" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="204" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="4"/>
     </row>
-    <row r="205" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="4"/>
     </row>
-    <row r="206" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="4"/>
     </row>
-    <row r="207" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="207" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="4"/>
     </row>
-    <row r="208" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="208" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="4"/>
     </row>
-    <row r="209" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="209" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="4"/>
     </row>
-    <row r="210" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="210" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="4"/>
     </row>
-    <row r="211" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="211" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="4"/>
     </row>
-    <row r="212" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="212" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="4"/>
     </row>
-    <row r="213" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="213" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="4"/>
     </row>
-    <row r="214" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="214" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="4"/>
     </row>
-    <row r="215" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="215" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="4"/>
     </row>
-    <row r="216" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="216" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="4"/>
     </row>
-    <row r="217" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="217" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="4"/>
     </row>
-    <row r="218" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="218" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="4"/>
     </row>
-    <row r="219" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="219" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="4"/>
     </row>
-    <row r="220" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="220" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="4"/>
     </row>
-    <row r="221" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="221" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="4"/>
     </row>
-    <row r="222" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="222" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="4"/>
     </row>
-    <row r="223" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="223" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="4"/>
     </row>
-    <row r="224" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="224" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="4"/>
     </row>
-    <row r="225" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="225" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="4"/>
     </row>
-    <row r="226" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="226" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="4"/>
     </row>
-    <row r="227" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="227" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="4"/>
     </row>
-    <row r="228" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="228" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="4"/>
     </row>
-    <row r="229" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="229" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="4"/>
     </row>
-    <row r="230" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="230" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="4"/>
     </row>
-    <row r="231" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="231" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="4"/>
     </row>
-    <row r="232" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="232" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="4"/>
     </row>
-    <row r="233" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="233" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="4"/>
     </row>
-    <row r="234" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="234" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="4"/>
     </row>
-    <row r="235" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="235" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="4"/>
     </row>
-    <row r="236" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="236" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="4"/>
     </row>
-    <row r="237" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="237" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="4"/>
     </row>
-    <row r="238" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="238" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="4"/>
     </row>
-    <row r="239" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="239" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="4"/>
     </row>
-    <row r="240" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="240" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="4"/>
     </row>
-    <row r="241" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="241" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="4"/>
     </row>
-    <row r="242" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="242" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="4"/>
     </row>
-    <row r="243" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="243" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="4"/>
     </row>
-    <row r="244" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="244" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="4"/>
     </row>
-    <row r="245" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="245" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="4"/>
     </row>
-    <row r="246" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="246" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="4"/>
     </row>
-    <row r="247" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="247" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="4"/>
     </row>
-    <row r="248" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="248" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="4"/>
     </row>
-    <row r="249" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="249" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="4"/>
     </row>
-    <row r="250" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="250" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="4"/>
     </row>
-    <row r="251" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="251" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="4"/>
     </row>
-    <row r="252" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="252" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="4"/>
     </row>
-    <row r="253" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="253" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="4"/>
     </row>
-    <row r="254" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="254" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="4"/>
     </row>
-    <row r="255" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="255" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A255" s="4"/>
     </row>
-    <row r="256" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="256" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="4"/>
     </row>
-    <row r="257" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="257" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="4"/>
     </row>
-    <row r="258" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="258" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A258" s="4"/>
     </row>
-    <row r="259" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="259" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="4"/>
     </row>
-    <row r="260" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="260" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A260" s="4"/>
     </row>
-    <row r="261" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="261" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="4"/>
     </row>
-    <row r="262" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="262" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="4"/>
     </row>
-    <row r="263" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="263" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="4"/>
     </row>
-    <row r="264" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="264" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="4"/>
     </row>
-    <row r="265" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="265" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A265" s="4"/>
     </row>
-    <row r="266" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="266" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="4"/>
     </row>
-    <row r="267" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="267" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="4"/>
     </row>
-    <row r="268" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="268" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="4"/>
     </row>
-    <row r="269" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="269" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="4"/>
     </row>
-    <row r="270" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="270" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="4"/>
     </row>
-    <row r="271" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="271" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="4"/>
     </row>
-    <row r="272" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="272" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="4"/>
     </row>
-    <row r="273" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="273" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A273" s="4"/>
     </row>
-    <row r="274" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="274" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A274" s="4"/>
     </row>
-    <row r="275" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="275" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A275" s="4"/>
     </row>
-    <row r="276" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="276" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A276" s="4"/>
     </row>
-    <row r="277" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="277" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A277" s="4"/>
     </row>
-    <row r="278" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="278" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="4"/>
     </row>
-    <row r="279" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="279" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A279" s="4"/>
     </row>
-    <row r="280" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="280" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A280" s="4"/>
     </row>
-    <row r="281" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="281" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A281" s="4"/>
     </row>
-    <row r="282" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="282" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A282" s="4"/>
     </row>
-    <row r="283" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="283" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A283" s="4"/>
     </row>
-    <row r="284" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="284" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A284" s="4"/>
     </row>
-    <row r="285" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="285" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A285" s="4"/>
     </row>
-    <row r="286" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="286" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A286" s="4"/>
     </row>
-    <row r="287" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="287" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A287" s="4"/>
     </row>
-    <row r="288" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="288" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A288" s="4"/>
     </row>
-    <row r="289" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="289" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A289" s="4"/>
     </row>
-    <row r="290" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="290" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A290" s="4"/>
     </row>
-    <row r="291" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="291" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A291" s="4"/>
     </row>
-    <row r="292" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="292" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A292" s="4"/>
     </row>
-    <row r="293" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="293" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A293" s="4"/>
     </row>
-    <row r="294" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="294" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A294" s="4"/>
     </row>
-    <row r="295" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="295" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A295" s="4"/>
     </row>
-    <row r="296" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="296" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A296" s="4"/>
     </row>
-    <row r="297" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="297" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A297" s="4"/>
     </row>
-    <row r="298" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="298" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A298" s="4"/>
     </row>
-    <row r="299" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="299" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A299" s="4"/>
     </row>
-    <row r="300" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="300" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A300" s="4"/>
     </row>
-    <row r="301" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="301" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A301" s="4"/>
     </row>
-    <row r="302" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="302" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A302" s="4"/>
     </row>
-    <row r="303" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="303" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A303" s="4"/>
     </row>
-    <row r="304" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="304" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A304" s="4"/>
     </row>
-    <row r="305" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="305" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A305" s="4"/>
     </row>
-    <row r="306" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="306" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A306" s="4"/>
     </row>
-    <row r="307" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="307" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A307" s="4"/>
     </row>
-    <row r="308" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="308" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A308" s="4"/>
     </row>
-    <row r="309" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="309" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A309" s="4"/>
     </row>
-    <row r="310" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="310" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A310" s="4"/>
     </row>
-    <row r="311" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="311" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A311" s="4"/>
     </row>
-    <row r="312" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="312" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A312" s="4"/>
     </row>
-    <row r="313" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="313" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A313" s="4"/>
     </row>
-    <row r="314" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="314" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A314" s="4"/>
     </row>
-    <row r="315" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="315" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A315" s="4"/>
     </row>
-    <row r="316" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="316" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A316" s="4"/>
     </row>
-    <row r="317" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="317" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A317" s="4"/>
     </row>
-    <row r="318" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="318" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A318" s="4"/>
     </row>
-    <row r="319" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="319" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A319" s="4"/>
     </row>
-    <row r="320" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="320" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A320" s="4"/>
     </row>
-    <row r="321" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="321" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A321" s="4"/>
     </row>
-    <row r="322" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="322" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A322" s="4"/>
     </row>
-    <row r="323" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="323" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A323" s="4"/>
     </row>
-    <row r="324" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="324" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A324" s="4"/>
     </row>
-    <row r="325" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="325" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A325" s="4"/>
     </row>
-    <row r="326" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="326" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A326" s="4"/>
     </row>
-    <row r="327" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="327" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A327" s="4"/>
     </row>
-    <row r="328" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="328" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A328" s="4"/>
     </row>
-    <row r="329" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="329" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A329" s="4"/>
     </row>
-    <row r="330" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="330" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A330" s="4"/>
     </row>
-    <row r="331" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="331" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A331" s="4"/>
     </row>
-    <row r="332" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="332" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A332" s="4"/>
     </row>
-    <row r="333" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="333" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A333" s="4"/>
     </row>
-    <row r="334" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="334" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A334" s="4"/>
     </row>
-    <row r="335" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="335" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A335" s="4"/>
     </row>
-    <row r="336" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="336" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A336" s="4"/>
     </row>
-    <row r="337" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="337" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A337" s="4"/>
     </row>
-    <row r="338" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="338" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A338" s="4"/>
     </row>
-    <row r="339" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="339" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A339" s="4"/>
     </row>
-    <row r="340" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="340" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A340" s="4"/>
     </row>
-    <row r="341" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="341" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A341" s="4"/>
     </row>
-    <row r="342" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="342" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A342" s="4"/>
     </row>
-    <row r="343" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="343" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A343" s="4"/>
     </row>
-    <row r="344" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="344" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A344" s="4"/>
     </row>
-    <row r="345" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="345" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A345" s="4"/>
     </row>
-    <row r="346" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="346" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A346" s="4"/>
     </row>
-    <row r="347" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="347" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A347" s="4"/>
     </row>
-    <row r="348" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="348" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A348" s="4"/>
     </row>
-    <row r="349" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="349" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A349" s="4"/>
     </row>
-    <row r="350" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="350" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A350" s="4"/>
     </row>
-    <row r="351" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="351" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A351" s="4"/>
     </row>
-    <row r="352" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="352" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A352" s="4"/>
     </row>
-    <row r="353" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="353" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A353" s="4"/>
     </row>
-    <row r="354" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="354" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A354" s="4"/>
     </row>
-    <row r="355" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="355" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A355" s="4"/>
     </row>
-    <row r="356" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="356" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A356" s="4"/>
     </row>
-    <row r="357" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="357" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A357" s="4"/>
     </row>
-    <row r="358" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="358" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A358" s="4"/>
     </row>
-    <row r="359" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="359" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A359" s="4"/>
     </row>
-    <row r="360" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="360" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A360" s="4"/>
     </row>
-    <row r="361" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="361" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A361" s="4"/>
     </row>
-    <row r="362" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="362" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A362" s="4"/>
     </row>
-    <row r="363" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="363" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A363" s="4"/>
     </row>
-    <row r="364" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="364" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A364" s="4"/>
     </row>
-    <row r="365" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="365" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A365" s="4"/>
     </row>
-    <row r="366" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="366" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A366" s="4"/>
     </row>
-    <row r="367" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="367" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A367" s="4"/>
     </row>
-    <row r="368" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="368" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A368" s="4"/>
     </row>
-    <row r="369" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="369" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A369" s="4"/>
     </row>
-    <row r="370" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="370" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A370" s="4"/>
     </row>
-    <row r="371" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="371" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A371" s="4"/>
     </row>
-    <row r="372" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="372" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A372" s="4"/>
     </row>
-    <row r="373" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="373" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A373" s="4"/>
     </row>
-    <row r="374" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="374" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A374" s="4"/>
     </row>
-    <row r="375" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="375" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A375" s="4"/>
     </row>
-    <row r="376" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="376" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A376" s="4"/>
     </row>
-    <row r="377" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="377" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A377" s="4"/>
     </row>
-    <row r="378" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="378" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A378" s="4"/>
     </row>
-    <row r="379" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="379" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A379" s="4"/>
     </row>
-    <row r="380" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="380" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A380" s="4"/>
     </row>
-    <row r="381" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="381" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A381" s="4"/>
     </row>
-    <row r="382" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="382" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A382" s="4"/>
     </row>
-    <row r="383" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="383" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A383" s="4"/>
     </row>
-    <row r="384" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="384" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A384" s="4"/>
     </row>
-    <row r="385" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="385" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A385" s="4"/>
     </row>
-    <row r="386" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="386" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A386" s="4"/>
     </row>
-    <row r="387" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="387" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A387" s="4"/>
     </row>
-    <row r="388" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="388" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A388" s="4"/>
     </row>
-    <row r="389" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="389" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A389" s="4"/>
     </row>
-    <row r="390" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="390" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A390" s="4"/>
     </row>
-    <row r="391" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="391" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A391" s="4"/>
     </row>
-    <row r="392" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="392" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A392" s="4"/>
     </row>
-    <row r="393" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="393" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A393" s="4"/>
     </row>
-    <row r="394" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="394" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A394" s="4"/>
     </row>
-    <row r="395" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="395" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A395" s="4"/>
     </row>
-    <row r="396" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="396" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A396" s="4"/>
     </row>
-    <row r="397" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="397" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A397" s="4"/>
     </row>
-    <row r="398" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="398" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A398" s="4"/>
     </row>
-    <row r="399" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="399" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A399" s="4"/>
     </row>
-    <row r="400" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="400" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A400" s="4"/>
     </row>
-    <row r="401" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="401" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A401" s="4"/>
     </row>
-    <row r="402" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="402" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A402" s="4"/>
     </row>
-    <row r="403" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="403" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A403" s="4"/>
     </row>
-    <row r="404" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="404" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A404" s="4"/>
     </row>
-    <row r="405" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="405" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A405" s="4"/>
     </row>
-    <row r="406" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="406" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A406" s="4"/>
     </row>
-    <row r="407" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="407" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A407" s="4"/>
     </row>
-    <row r="408" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="408" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A408" s="4"/>
     </row>
-    <row r="409" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="409" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A409" s="4"/>
     </row>
-    <row r="410" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="410" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A410" s="4"/>
     </row>
-    <row r="411" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="411" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A411" s="4"/>
     </row>
-    <row r="412" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="412" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A412" s="4"/>
     </row>
-    <row r="413" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="413" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A413" s="4"/>
     </row>
-    <row r="414" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="414" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A414" s="4"/>
     </row>
-    <row r="415" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="415" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A415" s="4"/>
     </row>
-    <row r="416" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="416" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A416" s="4"/>
     </row>
-    <row r="417" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="417" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A417" s="4"/>
     </row>
-    <row r="418" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="418" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A418" s="4"/>
     </row>
-    <row r="419" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="419" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A419" s="4"/>
     </row>
-    <row r="420" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="420" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A420" s="4"/>
     </row>
-    <row r="421" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="421" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A421" s="4"/>
     </row>
-    <row r="422" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="422" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A422" s="4"/>
     </row>
-    <row r="423" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="423" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A423" s="4"/>
     </row>
-    <row r="424" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="424" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A424" s="4"/>
     </row>
-    <row r="425" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="425" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A425" s="4"/>
     </row>
-    <row r="426" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="426" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A426" s="4"/>
     </row>
-    <row r="427" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="427" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A427" s="4"/>
     </row>
-    <row r="428" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="428" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A428" s="4"/>
     </row>
-    <row r="429" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="429" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A429" s="4"/>
     </row>
-    <row r="430" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="430" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A430" s="4"/>
     </row>
-    <row r="431" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="431" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A431" s="4"/>
     </row>
-    <row r="432" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="432" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A432" s="4"/>
     </row>
-    <row r="433" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="433" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A433" s="4"/>
     </row>
-    <row r="434" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="434" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A434" s="4"/>
     </row>
-    <row r="435" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="435" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A435" s="4"/>
     </row>
-    <row r="436" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="436" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A436" s="4"/>
     </row>
-    <row r="437" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="437" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A437" s="4"/>
     </row>
-    <row r="438" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="438" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A438" s="4"/>
     </row>
-    <row r="439" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="439" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A439" s="4"/>
     </row>
-    <row r="440" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="440" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A440" s="4"/>
     </row>
-    <row r="441" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="441" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A441" s="4"/>
     </row>
-    <row r="442" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="442" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A442" s="4"/>
     </row>
-    <row r="443" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="443" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A443" s="4"/>
     </row>
-    <row r="444" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="444" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A444" s="4"/>
     </row>
-    <row r="445" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="445" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A445" s="4"/>
     </row>
-    <row r="446" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="446" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A446" s="4"/>
     </row>
-    <row r="447" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="447" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A447" s="4"/>
     </row>
-    <row r="448" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="448" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A448" s="4"/>
     </row>
-    <row r="449" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="449" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A449" s="4"/>
     </row>
-    <row r="450" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="450" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A450" s="4"/>
     </row>
-    <row r="451" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="451" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A451" s="4"/>
     </row>
-    <row r="452" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="452" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A452" s="4"/>
     </row>
-    <row r="453" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="453" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A453" s="4"/>
     </row>
-    <row r="454" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="454" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A454" s="4"/>
     </row>
-    <row r="455" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="455" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A455" s="4"/>
     </row>
-    <row r="456" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="456" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A456" s="4"/>
     </row>
-    <row r="457" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="457" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A457" s="4"/>
     </row>
-    <row r="458" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="458" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A458" s="4"/>
     </row>
-    <row r="459" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="459" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A459" s="4"/>
     </row>
-    <row r="460" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="460" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A460" s="4"/>
     </row>
-    <row r="461" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="461" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A461" s="4"/>
     </row>
-    <row r="462" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="462" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A462" s="4"/>
     </row>
-    <row r="463" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="463" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A463" s="4"/>
     </row>
-    <row r="464" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="464" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A464" s="4"/>
     </row>
-    <row r="465" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="465" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A465" s="4"/>
     </row>
-    <row r="466" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="466" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A466" s="4"/>
     </row>
-    <row r="467" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="467" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A467" s="4"/>
     </row>
-    <row r="468" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="468" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A468" s="4"/>
     </row>
-    <row r="469" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="469" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A469" s="4"/>
     </row>
-    <row r="470" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="470" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A470" s="4"/>
     </row>
-    <row r="471" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="471" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A471" s="4"/>
     </row>
-    <row r="472" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="472" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A472" s="4"/>
     </row>
-    <row r="473" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="473" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A473" s="4"/>
     </row>
-    <row r="474" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="474" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A474" s="4"/>
     </row>
-    <row r="475" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="475" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A475" s="4"/>
     </row>
-    <row r="476" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="476" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A476" s="4"/>
     </row>
-    <row r="477" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="477" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A477" s="4"/>
     </row>
-    <row r="478" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="478" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A478" s="4"/>
     </row>
-    <row r="479" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="479" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A479" s="4"/>
     </row>
-    <row r="480" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="480" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A480" s="4"/>
     </row>
-    <row r="481" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="481" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A481" s="4"/>
     </row>
-    <row r="482" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="482" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A482" s="4"/>
     </row>
-    <row r="483" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="483" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A483" s="4"/>
     </row>
-    <row r="484" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="484" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A484" s="4"/>
     </row>
-    <row r="485" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="485" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A485" s="4"/>
     </row>
-    <row r="486" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="486" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A486" s="4"/>
     </row>
-    <row r="487" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="487" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A487" s="4"/>
     </row>
-    <row r="488" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="488" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A488" s="4"/>
     </row>
-    <row r="489" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="489" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A489" s="4"/>
     </row>
-    <row r="490" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="490" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A490" s="4"/>
     </row>
-    <row r="491" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="491" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A491" s="4"/>
     </row>
-    <row r="492" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="492" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A492" s="4"/>
     </row>
-    <row r="493" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="493" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A493" s="4"/>
     </row>
-    <row r="494" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="494" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A494" s="4"/>
     </row>
-    <row r="495" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="495" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A495" s="4"/>
     </row>
-    <row r="496" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="496" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A496" s="4"/>
     </row>
-    <row r="497" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="497" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A497" s="4"/>
     </row>
-    <row r="498" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="498" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A498" s="4"/>
     </row>
-    <row r="499" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="499" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A499" s="4"/>
     </row>
-    <row r="500" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="500" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A500" s="4"/>
     </row>
-    <row r="501" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="501" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A501" s="4"/>
     </row>
-    <row r="502" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="502" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A502" s="4"/>
     </row>
-    <row r="503" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="503" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A503" s="4"/>
     </row>
-    <row r="504" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="504" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A504" s="4"/>
     </row>
-    <row r="505" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="505" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A505" s="4"/>
     </row>
-    <row r="506" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="506" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A506" s="4"/>
     </row>
-    <row r="507" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="507" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A507" s="4"/>
     </row>
-    <row r="508" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="508" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A508" s="4"/>
     </row>
-    <row r="509" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="509" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A509" s="4"/>
     </row>
-    <row r="510" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="510" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A510" s="4"/>
     </row>
-    <row r="511" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="511" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A511" s="4"/>
     </row>
-    <row r="512" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="512" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A512" s="4"/>
     </row>
-    <row r="513" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="513" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A513" s="4"/>
     </row>
-    <row r="514" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="514" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A514" s="4"/>
     </row>
-    <row r="515" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="515" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A515" s="4"/>
     </row>
-    <row r="516" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="516" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A516" s="4"/>
     </row>
-    <row r="517" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="517" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A517" s="4"/>
     </row>
-    <row r="518" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="518" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A518" s="4"/>
     </row>
-    <row r="519" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="519" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A519" s="4"/>
     </row>
-    <row r="520" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="520" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A520" s="4"/>
     </row>
-    <row r="521" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="521" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A521" s="4"/>
     </row>
-    <row r="522" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="522" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A522" s="4"/>
     </row>
-    <row r="523" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="523" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A523" s="4"/>
     </row>
-    <row r="524" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="524" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A524" s="4"/>
     </row>
-    <row r="525" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="525" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A525" s="4"/>
     </row>
-    <row r="526" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="526" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A526" s="4"/>
     </row>
-    <row r="527" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="527" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A527" s="4"/>
     </row>
-    <row r="528" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="528" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A528" s="4"/>
     </row>
-    <row r="529" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="529" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A529" s="4"/>
     </row>
-    <row r="530" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="530" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A530" s="4"/>
     </row>
-    <row r="531" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="531" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A531" s="4"/>
     </row>
-    <row r="532" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="532" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A532" s="4"/>
     </row>
-    <row r="533" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="533" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A533" s="4"/>
     </row>
-    <row r="534" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="534" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A534" s="4"/>
     </row>
-    <row r="535" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="535" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A535" s="4"/>
     </row>
-    <row r="536" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="536" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A536" s="4"/>
     </row>
-    <row r="537" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="537" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A537" s="4"/>
     </row>
-    <row r="538" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="538" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A538" s="4"/>
     </row>
-    <row r="539" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="539" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A539" s="4"/>
     </row>
-    <row r="540" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="540" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A540" s="4"/>
     </row>
-    <row r="541" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="541" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A541" s="4"/>
     </row>
-    <row r="542" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="542" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A542" s="4"/>
     </row>
-    <row r="543" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="543" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A543" s="4"/>
     </row>
-    <row r="544" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="544" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A544" s="4"/>
     </row>
-    <row r="545" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="545" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A545" s="4"/>
     </row>
-    <row r="546" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="546" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A546" s="4"/>
     </row>
-    <row r="547" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="547" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A547" s="4"/>
     </row>
-    <row r="548" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="548" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A548" s="4"/>
     </row>
-    <row r="549" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="549" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A549" s="4"/>
     </row>
-    <row r="550" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="550" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A550" s="4"/>
     </row>
-    <row r="551" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="551" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A551" s="4"/>
     </row>
-    <row r="552" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="552" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A552" s="4"/>
     </row>
-    <row r="553" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="553" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A553" s="4"/>
     </row>
-    <row r="554" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="554" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A554" s="4"/>
     </row>
-    <row r="555" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="555" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A555" s="4"/>
     </row>
-    <row r="556" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="556" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A556" s="4"/>
     </row>
-    <row r="557" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="557" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A557" s="4"/>
     </row>
-    <row r="558" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="558" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A558" s="4"/>
     </row>
-    <row r="559" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="559" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A559" s="4"/>
     </row>
-    <row r="560" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="560" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A560" s="4"/>
     </row>
-    <row r="561" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="561" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A561" s="4"/>
     </row>
-    <row r="562" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="562" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A562" s="4"/>
     </row>
-    <row r="563" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="563" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A563" s="4"/>
     </row>
-    <row r="564" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="564" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A564" s="4"/>
     </row>
-    <row r="565" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="565" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A565" s="4"/>
     </row>
-    <row r="566" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="566" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A566" s="4"/>
     </row>
-    <row r="567" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="567" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A567" s="4"/>
     </row>
-    <row r="568" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="568" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A568" s="4"/>
     </row>
-    <row r="569" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="569" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A569" s="4"/>
     </row>
-    <row r="570" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="570" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A570" s="4"/>
     </row>
-    <row r="571" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="571" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A571" s="4"/>
     </row>
-    <row r="572" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="572" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A572" s="4"/>
     </row>
-    <row r="573" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="573" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A573" s="4"/>
     </row>
-    <row r="574" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="574" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A574" s="4"/>
     </row>
-    <row r="575" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="575" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A575" s="4"/>
     </row>
-    <row r="576" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="576" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A576" s="4"/>
     </row>
-    <row r="577" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="577" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A577" s="4"/>
     </row>
-    <row r="578" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="578" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A578" s="4"/>
     </row>
-    <row r="579" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="579" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A579" s="4"/>
     </row>
-    <row r="580" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="580" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A580" s="4"/>
     </row>
-    <row r="581" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="581" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A581" s="4"/>
     </row>
-    <row r="582" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="582" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A582" s="4"/>
     </row>
-    <row r="583" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="583" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A583" s="4"/>
     </row>
-    <row r="584" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="584" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A584" s="4"/>
     </row>
-    <row r="585" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="585" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A585" s="4"/>
     </row>
-    <row r="586" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="586" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A586" s="4"/>
     </row>
-    <row r="587" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="587" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A587" s="4"/>
     </row>
-    <row r="588" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="588" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A588" s="4"/>
     </row>
-    <row r="589" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="589" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A589" s="4"/>
     </row>
-    <row r="590" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="590" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A590" s="4"/>
     </row>
-    <row r="591" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="591" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A591" s="4"/>
     </row>
-    <row r="592" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="592" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A592" s="4"/>
     </row>
-    <row r="593" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="593" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A593" s="4"/>
     </row>
-    <row r="594" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="594" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A594" s="4"/>
     </row>
-    <row r="595" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="595" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A595" s="4"/>
     </row>
-    <row r="596" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="596" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A596" s="4"/>
     </row>
-    <row r="597" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="597" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A597" s="4"/>
     </row>
-    <row r="598" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="598" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A598" s="4"/>
     </row>
-    <row r="599" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="599" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A599" s="4"/>
     </row>
-    <row r="600" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="600" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A600" s="4"/>
     </row>
-    <row r="601" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="601" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A601" s="4"/>
     </row>
-    <row r="602" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="602" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A602" s="4"/>
     </row>
-    <row r="603" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="603" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A603" s="4"/>
     </row>
-    <row r="604" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="604" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A604" s="4"/>
     </row>
-    <row r="605" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="605" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A605" s="4"/>
     </row>
-    <row r="606" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="606" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A606" s="4"/>
     </row>
-    <row r="607" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="607" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A607" s="4"/>
     </row>
-    <row r="608" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="608" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A608" s="4"/>
     </row>
-    <row r="609" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="609" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A609" s="4"/>
     </row>
-    <row r="610" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="610" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A610" s="4"/>
     </row>
-    <row r="611" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="611" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A611" s="4"/>
     </row>
-    <row r="612" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="612" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A612" s="4"/>
     </row>
-    <row r="613" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="613" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A613" s="4"/>
     </row>
-    <row r="614" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="614" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A614" s="4"/>
     </row>
-    <row r="615" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="615" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A615" s="4"/>
     </row>
-    <row r="616" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="616" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A616" s="4"/>
     </row>
-    <row r="617" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="617" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A617" s="4"/>
     </row>
-    <row r="618" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="618" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A618" s="4"/>
     </row>
-    <row r="619" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="619" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A619" s="4"/>
     </row>
-    <row r="620" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="620" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A620" s="4"/>
     </row>
-    <row r="621" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="621" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A621" s="4"/>
     </row>
-    <row r="622" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="622" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A622" s="4"/>
     </row>
-    <row r="623" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="623" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A623" s="4"/>
     </row>
-    <row r="624" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="624" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A624" s="4"/>
     </row>
-    <row r="625" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="625" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A625" s="4"/>
     </row>
-    <row r="626" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="626" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A626" s="4"/>
     </row>
-    <row r="627" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="627" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A627" s="4"/>
     </row>
-    <row r="628" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="628" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A628" s="4"/>
     </row>
-    <row r="629" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="629" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A629" s="4"/>
     </row>
-    <row r="630" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="630" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A630" s="4"/>
     </row>
-    <row r="631" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="631" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A631" s="4"/>
     </row>
-    <row r="632" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="632" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A632" s="4"/>
     </row>
-    <row r="633" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="633" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A633" s="4"/>
     </row>
-    <row r="634" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="634" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A634" s="4"/>
     </row>
-    <row r="635" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="635" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A635" s="4"/>
     </row>
-    <row r="636" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="636" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A636" s="4"/>
     </row>
-    <row r="637" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="637" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A637" s="4"/>
     </row>
-    <row r="638" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="638" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A638" s="4"/>
     </row>
-    <row r="639" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="639" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A639" s="4"/>
     </row>
-    <row r="640" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="640" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A640" s="4"/>
     </row>
-    <row r="641" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="641" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A641" s="4"/>
     </row>
-    <row r="642" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="642" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A642" s="4"/>
     </row>
-    <row r="643" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="643" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A643" s="4"/>
     </row>
-    <row r="644" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="644" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A644" s="4"/>
     </row>
-    <row r="645" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="645" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A645" s="4"/>
     </row>
-    <row r="646" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="646" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A646" s="4"/>
     </row>
-    <row r="647" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="647" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A647" s="4"/>
     </row>
-    <row r="648" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="648" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A648" s="4"/>
     </row>
-    <row r="649" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="649" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A649" s="4"/>
     </row>
-    <row r="650" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="650" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A650" s="4"/>
     </row>
-    <row r="651" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="651" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A651" s="4"/>
     </row>
-    <row r="652" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="652" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A652" s="4"/>
     </row>
-    <row r="653" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="653" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A653" s="4"/>
     </row>
-    <row r="654" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="654" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A654" s="4"/>
     </row>
-    <row r="655" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="655" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A655" s="4"/>
     </row>
-    <row r="656" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="656" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A656" s="4"/>
     </row>
-    <row r="657" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="657" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A657" s="4"/>
     </row>
-    <row r="658" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="658" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A658" s="4"/>
     </row>
-    <row r="659" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="659" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A659" s="4"/>
     </row>
-    <row r="660" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="660" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A660" s="4"/>
     </row>
-    <row r="661" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="661" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A661" s="4"/>
     </row>
-    <row r="662" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="662" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A662" s="4"/>
     </row>
-    <row r="663" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="663" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A663" s="4"/>
     </row>
-    <row r="664" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="664" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A664" s="4"/>
     </row>
-    <row r="665" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="665" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A665" s="4"/>
     </row>
-    <row r="666" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="666" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A666" s="4"/>
     </row>
-    <row r="667" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="667" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A667" s="4"/>
     </row>
-    <row r="668" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="668" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A668" s="4"/>
     </row>
-    <row r="669" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="669" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A669" s="4"/>
     </row>
-    <row r="670" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="670" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A670" s="4"/>
     </row>
-    <row r="671" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="671" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A671" s="4"/>
     </row>
-    <row r="672" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="672" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A672" s="4"/>
     </row>
-    <row r="673" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="673" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A673" s="4"/>
     </row>
-    <row r="674" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="674" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A674" s="4"/>
     </row>
-    <row r="675" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="675" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A675" s="4"/>
     </row>
-    <row r="676" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="676" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A676" s="4"/>
     </row>
-    <row r="677" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="677" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A677" s="4"/>
     </row>
-    <row r="678" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="678" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A678" s="4"/>
     </row>
-    <row r="679" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="679" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A679" s="4"/>
     </row>
-    <row r="680" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="680" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A680" s="4"/>
     </row>
-    <row r="681" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="681" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A681" s="4"/>
     </row>
-    <row r="682" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="682" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A682" s="4"/>
     </row>
-    <row r="683" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="683" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A683" s="4"/>
     </row>
-    <row r="684" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="684" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A684" s="4"/>
     </row>
-    <row r="685" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="685" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A685" s="4"/>
     </row>
-    <row r="686" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="686" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A686" s="4"/>
     </row>
-    <row r="687" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="687" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A687" s="4"/>
     </row>
-    <row r="688" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="688" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A688" s="4"/>
     </row>
-    <row r="689" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="689" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A689" s="4"/>
     </row>
-    <row r="690" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="690" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A690" s="4"/>
     </row>
-    <row r="691" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="691" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A691" s="4"/>
     </row>
-    <row r="692" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="692" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A692" s="4"/>
     </row>
-    <row r="693" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="693" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A693" s="4"/>
     </row>
-    <row r="694" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="694" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A694" s="4"/>
     </row>
-    <row r="695" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="695" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A695" s="4"/>
     </row>
-    <row r="696" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="696" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A696" s="4"/>
     </row>
-    <row r="697" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="697" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A697" s="4"/>
     </row>
-    <row r="698" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="698" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A698" s="4"/>
     </row>
-    <row r="699" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="699" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A699" s="4"/>
     </row>
-    <row r="700" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="700" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A700" s="4"/>
     </row>
-    <row r="701" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="701" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A701" s="4"/>
     </row>
-    <row r="702" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="702" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A702" s="4"/>
     </row>
-    <row r="703" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="703" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A703" s="4"/>
     </row>
-    <row r="704" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="704" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A704" s="4"/>
     </row>
-    <row r="705" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="705" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A705" s="4"/>
     </row>
-    <row r="706" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="706" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A706" s="4"/>
     </row>
-    <row r="707" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="707" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A707" s="4"/>
     </row>
-    <row r="708" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="708" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A708" s="4"/>
     </row>
-    <row r="709" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="709" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A709" s="4"/>
     </row>
-    <row r="710" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="710" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A710" s="4"/>
     </row>
-    <row r="711" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="711" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A711" s="4"/>
     </row>
-    <row r="712" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="712" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A712" s="4"/>
     </row>
-    <row r="713" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="713" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A713" s="4"/>
     </row>
-    <row r="714" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="714" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A714" s="4"/>
     </row>
-    <row r="715" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="715" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A715" s="4"/>
     </row>
-    <row r="716" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="716" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A716" s="4"/>
     </row>
-    <row r="717" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="717" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A717" s="4"/>
     </row>
-    <row r="718" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="718" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A718" s="4"/>
     </row>
-    <row r="719" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="719" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A719" s="4"/>
     </row>
-    <row r="720" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="720" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A720" s="4"/>
     </row>
-    <row r="721" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="721" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A721" s="4"/>
     </row>
-    <row r="722" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="722" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A722" s="4"/>
     </row>
-    <row r="723" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="723" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A723" s="4"/>
     </row>
-    <row r="724" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="724" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A724" s="4"/>
     </row>
-    <row r="725" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="725" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A725" s="4"/>
     </row>
-    <row r="726" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="726" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A726" s="4"/>
     </row>
-    <row r="727" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="727" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A727" s="4"/>
     </row>
-    <row r="728" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="728" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A728" s="4"/>
     </row>
-    <row r="729" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="729" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A729" s="4"/>
     </row>
-    <row r="730" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="730" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A730" s="4"/>
     </row>
-    <row r="731" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="731" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A731" s="4"/>
     </row>
-    <row r="732" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="732" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A732" s="4"/>
     </row>
-    <row r="733" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="733" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A733" s="4"/>
     </row>
-    <row r="734" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="734" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A734" s="4"/>
     </row>
-    <row r="735" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="735" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A735" s="4"/>
     </row>
-    <row r="736" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="736" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A736" s="4"/>
     </row>
-    <row r="737" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="737" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A737" s="4"/>
     </row>
-    <row r="738" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="738" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A738" s="4"/>
     </row>
-    <row r="739" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="739" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A739" s="4"/>
     </row>
-    <row r="740" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="740" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A740" s="4"/>
     </row>
-    <row r="741" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="741" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A741" s="4"/>
     </row>
-    <row r="742" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="742" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A742" s="4"/>
     </row>
-    <row r="743" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="743" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A743" s="4"/>
     </row>
-    <row r="744" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="744" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A744" s="4"/>
     </row>
-    <row r="745" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="745" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A745" s="4"/>
     </row>
-    <row r="746" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="746" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A746" s="4"/>
     </row>
-    <row r="747" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="747" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A747" s="4"/>
     </row>
-    <row r="748" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="748" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A748" s="4"/>
     </row>
-    <row r="749" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="749" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A749" s="4"/>
     </row>
-    <row r="750" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="750" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A750" s="4"/>
     </row>
-    <row r="751" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="751" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A751" s="4"/>
     </row>
-    <row r="752" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="752" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A752" s="4"/>
     </row>
-    <row r="753" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="753" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A753" s="4"/>
     </row>
-    <row r="754" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="754" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A754" s="4"/>
     </row>
-    <row r="755" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="755" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A755" s="4"/>
     </row>
-    <row r="756" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="756" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A756" s="4"/>
     </row>
-    <row r="757" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="757" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A757" s="4"/>
     </row>
-    <row r="758" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="758" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A758" s="4"/>
     </row>
-    <row r="759" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="759" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A759" s="4"/>
     </row>
-    <row r="760" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="760" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A760" s="4"/>
     </row>
-    <row r="761" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="761" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A761" s="4"/>
     </row>
-    <row r="762" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="762" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A762" s="4"/>
     </row>
-    <row r="763" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="763" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A763" s="4"/>
     </row>
-    <row r="764" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="764" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A764" s="4"/>
     </row>
-    <row r="765" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="765" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A765" s="4"/>
     </row>
-    <row r="766" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="766" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A766" s="4"/>
     </row>
-    <row r="767" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="767" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A767" s="4"/>
     </row>
-    <row r="768" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="768" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A768" s="4"/>
     </row>
-    <row r="769" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="769" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A769" s="4"/>
     </row>
-    <row r="770" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="770" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A770" s="4"/>
     </row>
-    <row r="771" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="771" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A771" s="4"/>
     </row>
-    <row r="772" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="772" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A772" s="4"/>
     </row>
-    <row r="773" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="773" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A773" s="4"/>
     </row>
-    <row r="774" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="774" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A774" s="4"/>
     </row>
-    <row r="775" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="775" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A775" s="4"/>
     </row>
-    <row r="776" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="776" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A776" s="4"/>
     </row>
-    <row r="777" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="777" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A777" s="4"/>
     </row>
-    <row r="778" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="778" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A778" s="4"/>
     </row>
-    <row r="779" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="779" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A779" s="4"/>
     </row>
-    <row r="780" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="780" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A780" s="4"/>
     </row>
-    <row r="781" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="781" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A781" s="4"/>
     </row>
-    <row r="782" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="782" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A782" s="4"/>
     </row>
-    <row r="783" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="783" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A783" s="4"/>
     </row>
-    <row r="784" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="784" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A784" s="4"/>
     </row>
-    <row r="785" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="785" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A785" s="4"/>
     </row>
-    <row r="786" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="786" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A786" s="4"/>
     </row>
-    <row r="787" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="787" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A787" s="4"/>
     </row>
-    <row r="788" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="788" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A788" s="4"/>
     </row>
-    <row r="789" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="789" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A789" s="4"/>
     </row>
-    <row r="790" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="790" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A790" s="4"/>
     </row>
-    <row r="791" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="791" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A791" s="4"/>
     </row>
-    <row r="792" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="792" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A792" s="4"/>
     </row>
-    <row r="793" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="793" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A793" s="4"/>
     </row>
-    <row r="794" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="794" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A794" s="4"/>
     </row>
-    <row r="795" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="795" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A795" s="4"/>
     </row>
-    <row r="796" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="796" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A796" s="4"/>
     </row>
-    <row r="797" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="797" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A797" s="4"/>
     </row>
-    <row r="798" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="798" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A798" s="4"/>
     </row>
-    <row r="799" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="799" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A799" s="4"/>
     </row>
-    <row r="800" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="800" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A800" s="4"/>
     </row>
-    <row r="801" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="801" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A801" s="4"/>
     </row>
-    <row r="802" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="802" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A802" s="4"/>
     </row>
-    <row r="803" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="803" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A803" s="4"/>
     </row>
-    <row r="804" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="804" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A804" s="4"/>
     </row>
-    <row r="805" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="805" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A805" s="4"/>
     </row>
-    <row r="806" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="806" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A806" s="4"/>
     </row>
-    <row r="807" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="807" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A807" s="4"/>
     </row>
-    <row r="808" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="808" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A808" s="4"/>
     </row>
-    <row r="809" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="809" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A809" s="4"/>
     </row>
-    <row r="810" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="810" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A810" s="4"/>
     </row>
-    <row r="811" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="811" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A811" s="4"/>
     </row>
-    <row r="812" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="812" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A812" s="4"/>
     </row>
-    <row r="813" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="813" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A813" s="4"/>
     </row>
-    <row r="814" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="814" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A814" s="4"/>
     </row>
-    <row r="815" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="815" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A815" s="4"/>
     </row>
-    <row r="816" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="816" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A816" s="4"/>
     </row>
-    <row r="817" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="817" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A817" s="4"/>
     </row>
-    <row r="818" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="818" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A818" s="4"/>
     </row>
-    <row r="819" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="819" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A819" s="4"/>
     </row>
-    <row r="820" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="820" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A820" s="4"/>
     </row>
-    <row r="821" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="821" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A821" s="4"/>
     </row>
-    <row r="822" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="822" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A822" s="4"/>
     </row>
-    <row r="823" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="823" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A823" s="4"/>
     </row>
-    <row r="824" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="824" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A824" s="4"/>
     </row>
-    <row r="825" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="825" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A825" s="4"/>
     </row>
-    <row r="826" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="826" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A826" s="4"/>
     </row>
-    <row r="827" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="827" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A827" s="4"/>
     </row>
-    <row r="828" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="828" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A828" s="4"/>
     </row>
-    <row r="829" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="829" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A829" s="4"/>
     </row>
-    <row r="830" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="830" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A830" s="4"/>
     </row>
-    <row r="831" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="831" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A831" s="4"/>
     </row>
-    <row r="832" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="832" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A832" s="4"/>
     </row>
-    <row r="833" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="833" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A833" s="4"/>
     </row>
-    <row r="834" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="834" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A834" s="4"/>
     </row>
-    <row r="835" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="835" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A835" s="4"/>
     </row>
-    <row r="836" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="836" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A836" s="4"/>
     </row>
-    <row r="837" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="837" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A837" s="4"/>
     </row>
-    <row r="838" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="838" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A838" s="4"/>
     </row>
-    <row r="839" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="839" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A839" s="4"/>
     </row>
-    <row r="840" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="840" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A840" s="4"/>
     </row>
-    <row r="841" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="841" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A841" s="4"/>
     </row>
-    <row r="842" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="842" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A842" s="4"/>
     </row>
-    <row r="843" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="843" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A843" s="4"/>
     </row>
-    <row r="844" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="844" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A844" s="4"/>
     </row>
-    <row r="845" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="845" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A845" s="4"/>
     </row>
-    <row r="846" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="846" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A846" s="4"/>
     </row>
-    <row r="847" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="847" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A847" s="4"/>
     </row>
-    <row r="848" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="848" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A848" s="4"/>
     </row>
-    <row r="849" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="849" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A849" s="4"/>
     </row>
-    <row r="850" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="850" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A850" s="4"/>
     </row>
-    <row r="851" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="851" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A851" s="4"/>
     </row>
-    <row r="852" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="852" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A852" s="4"/>
     </row>
-    <row r="853" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="853" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A853" s="4"/>
     </row>
-    <row r="854" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="854" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A854" s="4"/>
     </row>
-    <row r="855" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="855" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A855" s="4"/>
     </row>
-    <row r="856" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="856" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A856" s="4"/>
     </row>
-    <row r="857" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="857" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A857" s="4"/>
     </row>
-    <row r="858" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="858" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A858" s="4"/>
     </row>
-    <row r="859" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="859" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A859" s="4"/>
     </row>
-    <row r="860" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="860" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A860" s="4"/>
     </row>
-    <row r="861" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="861" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A861" s="4"/>
     </row>
-    <row r="862" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="862" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A862" s="4"/>
     </row>
-    <row r="863" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="863" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A863" s="4"/>
     </row>
-    <row r="864" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="864" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A864" s="4"/>
     </row>
-    <row r="865" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="865" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A865" s="4"/>
     </row>
-    <row r="866" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="866" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A866" s="4"/>
     </row>
-    <row r="867" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="867" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A867" s="4"/>
     </row>
-    <row r="868" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="868" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A868" s="4"/>
     </row>
-    <row r="869" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="869" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A869" s="4"/>
     </row>
-    <row r="870" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="870" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A870" s="4"/>
     </row>
-    <row r="871" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="871" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A871" s="4"/>
     </row>
-    <row r="872" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="872" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A872" s="4"/>
     </row>
-    <row r="873" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="873" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A873" s="4"/>
     </row>
-    <row r="874" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="874" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A874" s="4"/>
     </row>
-    <row r="875" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="875" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A875" s="4"/>
     </row>
-    <row r="876" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="876" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A876" s="4"/>
     </row>
-    <row r="877" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="877" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A877" s="4"/>
     </row>
-    <row r="878" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="878" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A878" s="4"/>
     </row>
-    <row r="879" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="879" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A879" s="4"/>
     </row>
-    <row r="880" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="880" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A880" s="4"/>
     </row>
-    <row r="881" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="881" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A881" s="4"/>
     </row>
-    <row r="882" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="882" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A882" s="4"/>
     </row>
-    <row r="883" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="883" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A883" s="4"/>
     </row>
-    <row r="884" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="884" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A884" s="4"/>
     </row>
-    <row r="885" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="885" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A885" s="4"/>
     </row>
-    <row r="886" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="886" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A886" s="4"/>
     </row>
-    <row r="887" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="887" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A887" s="4"/>
     </row>
-    <row r="888" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="888" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A888" s="4"/>
     </row>
-    <row r="889" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="889" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A889" s="4"/>
     </row>
-    <row r="890" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="890" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A890" s="4"/>
     </row>
-    <row r="891" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="891" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A891" s="4"/>
     </row>
-    <row r="892" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="892" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A892" s="4"/>
     </row>
-    <row r="893" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="893" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A893" s="4"/>
     </row>
-    <row r="894" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="894" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A894" s="4"/>
     </row>
-    <row r="895" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="895" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A895" s="4"/>
     </row>
-    <row r="896" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="896" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A896" s="4"/>
     </row>
-    <row r="897" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="897" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A897" s="4"/>
     </row>
-    <row r="898" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="898" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A898" s="4"/>
     </row>
-    <row r="899" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="899" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A899" s="4"/>
     </row>
-    <row r="900" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="900" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A900" s="4"/>
     </row>
-    <row r="901" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="901" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A901" s="4"/>
     </row>
-    <row r="902" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="902" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A902" s="4"/>
     </row>
-    <row r="903" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="903" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A903" s="4"/>
     </row>
-    <row r="904" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="904" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A904" s="4"/>
     </row>
-    <row r="905" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="905" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A905" s="4"/>
     </row>
-    <row r="906" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="906" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A906" s="4"/>
     </row>
-    <row r="907" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="907" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A907" s="4"/>
     </row>
-    <row r="908" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="908" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A908" s="4"/>
     </row>
-    <row r="909" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="909" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A909" s="4"/>
     </row>
-    <row r="910" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="910" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A910" s="4"/>
     </row>
-    <row r="911" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="911" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A911" s="4"/>
     </row>
-    <row r="912" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="912" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A912" s="4"/>
     </row>
-    <row r="913" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="913" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A913" s="4"/>
     </row>
-    <row r="914" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="914" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A914" s="4"/>
     </row>
-    <row r="915" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="915" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A915" s="4"/>
     </row>
-    <row r="916" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="916" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A916" s="4"/>
     </row>
-    <row r="917" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="917" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A917" s="4"/>
     </row>
-    <row r="918" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="918" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A918" s="4"/>
     </row>
-    <row r="919" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="919" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A919" s="4"/>
     </row>
-    <row r="920" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="920" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A920" s="4"/>
     </row>
-    <row r="921" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="921" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A921" s="4"/>
     </row>
-    <row r="922" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="922" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A922" s="4"/>
     </row>
-    <row r="923" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="923" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A923" s="4"/>
     </row>
-    <row r="924" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="924" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A924" s="4"/>
     </row>
-    <row r="925" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="925" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A925" s="4"/>
     </row>
-    <row r="926" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="926" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A926" s="4"/>
     </row>
-    <row r="927" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="927" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A927" s="4"/>
     </row>
-    <row r="928" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="928" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A928" s="4"/>
     </row>
-    <row r="929" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="929" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A929" s="4"/>
     </row>
-    <row r="930" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="930" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A930" s="4"/>
     </row>
-    <row r="931" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="931" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A931" s="4"/>
     </row>
-    <row r="932" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="932" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A932" s="4"/>
     </row>
-    <row r="933" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="933" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A933" s="4"/>
     </row>
-    <row r="934" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="934" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A934" s="4"/>
     </row>
-    <row r="935" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="935" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A935" s="4"/>
     </row>
-    <row r="936" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="936" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A936" s="4"/>
     </row>
-    <row r="937" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="937" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A937" s="4"/>
     </row>
-    <row r="938" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="938" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A938" s="4"/>
     </row>
-    <row r="939" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="939" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A939" s="4"/>
     </row>
-    <row r="940" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="940" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A940" s="4"/>
     </row>
-    <row r="941" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="941" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A941" s="4"/>
     </row>
-    <row r="942" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="942" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A942" s="4"/>
     </row>
-    <row r="943" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="943" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A943" s="4"/>
     </row>
-    <row r="944" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="944" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A944" s="4"/>
     </row>
-    <row r="945" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="945" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A945" s="4"/>
     </row>
-    <row r="946" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="946" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A946" s="4"/>
     </row>
-    <row r="947" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="947" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A947" s="4"/>
     </row>
-    <row r="948" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="948" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A948" s="4"/>
     </row>
-    <row r="949" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="949" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A949" s="4"/>
     </row>
-    <row r="950" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="950" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A950" s="4"/>
     </row>
-    <row r="951" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="951" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A951" s="4"/>
     </row>
-    <row r="952" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="952" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A952" s="4"/>
     </row>
-    <row r="953" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="953" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A953" s="4"/>
     </row>
-    <row r="954" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="954" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A954" s="4"/>
     </row>
-    <row r="955" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="955" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A955" s="4"/>
     </row>
-    <row r="956" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="956" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A956" s="4"/>
     </row>
-    <row r="957" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="957" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A957" s="4"/>
     </row>
-    <row r="958" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="958" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A958" s="4"/>
     </row>
-    <row r="959" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="959" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A959" s="4"/>
     </row>
-    <row r="960" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="960" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A960" s="4"/>
     </row>
-    <row r="961" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="961" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A961" s="4"/>
     </row>
-    <row r="962" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="962" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A962" s="4"/>
     </row>
-    <row r="963" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="963" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A963" s="4"/>
     </row>
-    <row r="964" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="964" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A964" s="4"/>
     </row>
-    <row r="965" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="965" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A965" s="4"/>
     </row>
-    <row r="966" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="966" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A966" s="4"/>
     </row>
-    <row r="967" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="967" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A967" s="4"/>
     </row>
-    <row r="968" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="968" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A968" s="4"/>
     </row>
-    <row r="969" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="969" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A969" s="4"/>
     </row>
-    <row r="970" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="970" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A970" s="4"/>
     </row>
-    <row r="971" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="971" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A971" s="4"/>
     </row>
-    <row r="972" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="972" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A972" s="4"/>
     </row>
-    <row r="973" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="973" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A973" s="4"/>
     </row>
-    <row r="974" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="974" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A974" s="4"/>
     </row>
-    <row r="975" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="975" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A975" s="4"/>
     </row>
-    <row r="976" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="976" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A976" s="4"/>
     </row>
-    <row r="977" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="977" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A977" s="4"/>
     </row>
-    <row r="978" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="978" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A978" s="4"/>
     </row>
-    <row r="979" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="979" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A979" s="4"/>
     </row>
-    <row r="980" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="980" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A980" s="4"/>
     </row>
-    <row r="981" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="981" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A981" s="4"/>
     </row>
-    <row r="982" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="982" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A982" s="4"/>
     </row>
-    <row r="983" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="983" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A983" s="4"/>
     </row>
-    <row r="984" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="984" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A984" s="4"/>
     </row>
-    <row r="985" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="985" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A985" s="4"/>
     </row>
-    <row r="986" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="986" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A986" s="4"/>
     </row>
-    <row r="987" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="987" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A987" s="4"/>
     </row>
-    <row r="988" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="988" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A988" s="4"/>
     </row>
-    <row r="989" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="989" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A989" s="4"/>
     </row>
-    <row r="990" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="990" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A990" s="4"/>
     </row>
-    <row r="991" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="991" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A991" s="4"/>
     </row>
-    <row r="992" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="992" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A992" s="4"/>
     </row>
-    <row r="993" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="993" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A993" s="4"/>
     </row>
-    <row r="994" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="994" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A994" s="4"/>
     </row>
-    <row r="995" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="995" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A995" s="4"/>
     </row>
-    <row r="996" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="996" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A996" s="4"/>
     </row>
-    <row r="997" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="997" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A997" s="4"/>
     </row>
-    <row r="998" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="998" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A998" s="4"/>
     </row>
-    <row r="999" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="999" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A999" s="4"/>
-    </row>
-    <row r="1000" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1000" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>